<commit_message>
changed series for unemployment rate
</commit_message>
<xml_diff>
--- a/data/inflation_DK_MONAlong.xlsx
+++ b/data/inflation_DK_MONAlong.xlsx
@@ -1161,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1715,7 +1715,7 @@
         <v>2764.9462199999998</v>
       </c>
       <c r="E19" s="2">
-        <v>9.6068060231565742</v>
+        <v>10.530385654492184</v>
       </c>
       <c r="F19" s="2">
         <v>27.237580000000001</v>
@@ -1738,7 +1738,7 @@
         <v>2773.60034</v>
       </c>
       <c r="E20" s="2">
-        <v>9.2543776512516569</v>
+        <v>10.133071317212689</v>
       </c>
       <c r="F20" s="2">
         <v>26.540880000000001</v>
@@ -1761,7 +1761,7 @@
         <v>2780.2424500000002</v>
       </c>
       <c r="E21" s="2">
-        <v>8.7896751594451761</v>
+        <v>9.6190783614504305</v>
       </c>
       <c r="F21" s="2">
         <v>26.540880000000001</v>
@@ -1784,7 +1784,7 @@
         <v>2779.3887500000001</v>
       </c>
       <c r="E22" s="2">
-        <v>8.2335222087950086</v>
+        <v>9.0141510528321955</v>
       </c>
       <c r="F22" s="2">
         <v>27.469809999999999</v>
@@ -1807,7 +1807,7 @@
         <v>2793.8634499999998</v>
       </c>
       <c r="E23" s="2">
-        <v>7.863140555419772</v>
+        <v>8.582677866990478</v>
       </c>
       <c r="F23" s="2">
         <v>17.782389999999999</v>
@@ -1830,7 +1830,7 @@
         <v>2801.8074099999999</v>
       </c>
       <c r="E24" s="2">
-        <v>7.7096466098645937</v>
+        <v>8.3915867677045721</v>
       </c>
       <c r="F24" s="2">
         <v>12.706440000000001</v>
@@ -1853,7 +1853,7 @@
         <v>2799.2087099999999</v>
       </c>
       <c r="E25" s="2">
-        <v>7.6808645683300982</v>
+        <v>8.339713968363121</v>
       </c>
       <c r="F25" s="2">
         <v>12.37468</v>
@@ -1876,7 +1876,7 @@
         <v>2806.5557399999998</v>
       </c>
       <c r="E26" s="2">
-        <v>7.6417274363487264</v>
+        <v>8.2851872990065196</v>
       </c>
       <c r="F26" s="2">
         <v>14.630660000000001</v>
@@ -1899,7 +1899,7 @@
         <v>2802.7570500000002</v>
       </c>
       <c r="E27" s="2">
-        <v>7.750618270677438</v>
+        <v>8.3902420267249926</v>
       </c>
       <c r="F27" s="2">
         <v>17.616510000000002</v>
@@ -1922,7 +1922,7 @@
         <v>2815.3772399999998</v>
       </c>
       <c r="E28" s="2">
-        <v>7.7558743069188143</v>
+        <v>8.382198185141899</v>
       </c>
       <c r="F28" s="2">
         <v>18.578620000000001</v>
@@ -1945,7 +1945,7 @@
         <v>2819.57341</v>
       </c>
       <c r="E29" s="2">
-        <v>7.7107167782519275</v>
+        <v>8.3192620232862602</v>
       </c>
       <c r="F29" s="2">
         <v>18.91038</v>
@@ -1968,7 +1968,7 @@
         <v>2828.3074299999998</v>
       </c>
       <c r="E30" s="2">
-        <v>7.743506511242308</v>
+        <v>8.3297345054424525</v>
       </c>
       <c r="F30" s="2">
         <v>17.815570000000001</v>
@@ -1991,7 +1991,7 @@
         <v>2815.5081500000001</v>
       </c>
       <c r="E31" s="2">
-        <v>8.2236316737353441</v>
+        <v>8.7990404175172277</v>
       </c>
       <c r="F31" s="2">
         <v>15.72547</v>
@@ -2014,7 +2014,7 @@
         <v>2818.7068599999998</v>
       </c>
       <c r="E32" s="2">
-        <v>8.3279522014573732</v>
+        <v>8.9058640161894296</v>
       </c>
       <c r="F32" s="2">
         <v>16.25629</v>
@@ -2037,7 +2037,7 @@
         <v>2817.3361399999999</v>
       </c>
       <c r="E33" s="2">
-        <v>8.3996782151809537</v>
+        <v>9.0090527803900198</v>
       </c>
       <c r="F33" s="2">
         <v>14.36525</v>
@@ -2060,7 +2060,7 @@
         <v>2836.0019600000001</v>
       </c>
       <c r="E34" s="2">
-        <v>8.9937709351935702</v>
+        <v>9.6577471943051751</v>
       </c>
       <c r="F34" s="2">
         <v>13.303610000000001</v>
@@ -2083,7 +2083,7 @@
         <v>2834.6161900000002</v>
       </c>
       <c r="E35" s="2">
-        <v>9.212055265937078</v>
+        <v>9.9491317562613766</v>
       </c>
       <c r="F35" s="2">
         <v>16.551559999999998</v>
@@ -2106,7 +2106,7 @@
         <v>2833.9809700000001</v>
       </c>
       <c r="E36" s="2">
-        <v>9.2876851604264647</v>
+        <v>10.103497617087788</v>
       </c>
       <c r="F36" s="2">
         <v>18.353020000000001</v>
@@ -2129,7 +2129,7 @@
         <v>2829.9927200000002</v>
       </c>
       <c r="E37" s="2">
-        <v>9.2638372582103319</v>
+        <v>10.151580885528883</v>
       </c>
       <c r="F37" s="2">
         <v>17.40418</v>
@@ -2152,7 +2152,7 @@
         <v>2845.0467600000002</v>
       </c>
       <c r="E38" s="2">
-        <v>9.2615982171062807</v>
+        <v>10.203322643477094</v>
       </c>
       <c r="F38" s="2">
         <v>18.953510000000001</v>
@@ -2175,7 +2175,7 @@
         <v>2839.72676</v>
       </c>
       <c r="E39" s="2">
-        <v>9.3034781980221215</v>
+        <v>10.303142686868931</v>
       </c>
       <c r="F39" s="2">
         <v>19.392759999999999</v>
@@ -2198,7 +2198,7 @@
         <v>2820.7603199999999</v>
       </c>
       <c r="E40" s="2">
-        <v>9.4893783814996393</v>
+        <v>10.545780791471145</v>
       </c>
       <c r="F40" s="2">
         <v>16.706489999999999</v>
@@ -2221,7 +2221,7 @@
         <v>2825.0945499999998</v>
       </c>
       <c r="E41" s="2">
-        <v>9.7345149032268683</v>
+        <v>10.841141582323324</v>
       </c>
       <c r="F41" s="2">
         <v>25.432469999999999</v>
@@ -2244,7 +2244,7 @@
         <v>2854.0498899999998</v>
       </c>
       <c r="E42" s="2">
-        <v>9.8085597936061326</v>
+        <v>10.957776214626719</v>
       </c>
       <c r="F42" s="2">
         <v>30.91018</v>
@@ -2267,7 +2267,7 @@
         <v>2816.3233700000001</v>
       </c>
       <c r="E43" s="2">
-        <v>10.162624542649731</v>
+        <v>11.382758933680263</v>
       </c>
       <c r="F43" s="2">
         <v>19.938839999999999</v>
@@ -2290,7 +2290,7 @@
         <v>2823.1937600000001</v>
       </c>
       <c r="E44" s="2">
-        <v>10.420813624921019</v>
+        <v>11.723481565076852</v>
       </c>
       <c r="F44" s="2">
         <v>18.917020000000001</v>
@@ -2313,7 +2313,7 @@
         <v>2839.9344299999998</v>
       </c>
       <c r="E45" s="2">
-        <v>10.559413866467333</v>
+        <v>11.917342049337387</v>
       </c>
       <c r="F45" s="2">
         <v>19.79618</v>
@@ -2336,7 +2336,7 @@
         <v>2874.9150800000002</v>
       </c>
       <c r="E46" s="2">
-        <v>10.729641447357114</v>
+        <v>12.068993008308263</v>
       </c>
       <c r="F46" s="2">
         <v>20.373449999999998</v>
@@ -2359,7 +2359,7 @@
         <v>2837.8703300000002</v>
       </c>
       <c r="E47" s="2">
-        <v>10.947974849858625</v>
+        <v>12.336285992320162</v>
       </c>
       <c r="F47" s="2">
         <v>17.81889</v>
@@ -2382,7 +2382,7 @@
         <v>2834.8643099999999</v>
       </c>
       <c r="E48" s="2">
-        <v>11.083186905690029</v>
+        <v>12.441054012916759</v>
       </c>
       <c r="F48" s="2">
         <v>19.839310000000001</v>
@@ -2405,7 +2405,7 @@
         <v>2834.3765100000001</v>
       </c>
       <c r="E49" s="2">
-        <v>11.187381382863634</v>
+        <v>12.581458346901131</v>
       </c>
       <c r="F49" s="2">
         <v>20.111350000000002</v>
@@ -2428,7 +2428,7 @@
         <v>2841.0887600000001</v>
       </c>
       <c r="E50" s="2">
-        <v>11.597200504217966</v>
+        <v>13.024137267714227</v>
       </c>
       <c r="F50" s="2">
         <v>19.195689999999999</v>
@@ -2451,7 +2451,7 @@
         <v>2842.45705</v>
       </c>
       <c r="E51" s="2">
-        <v>11.991669320034228</v>
+        <v>13.480499204024909</v>
       </c>
       <c r="F51" s="2">
         <v>18.267109999999999</v>
@@ -2474,7 +2474,7 @@
         <v>2827.0625399999999</v>
       </c>
       <c r="E52" s="2">
-        <v>12.243504878388716</v>
+        <v>13.848176135502118</v>
       </c>
       <c r="F52" s="2">
         <v>18.51193</v>
@@ -2497,7 +2497,7 @@
         <v>2809.3939700000001</v>
       </c>
       <c r="E53" s="2">
-        <v>12.231320123464206</v>
+        <v>13.927950446907236</v>
       </c>
       <c r="F53" s="2">
         <v>16.679030000000001</v>
@@ -2520,7 +2520,7 @@
         <v>2798.7609400000001</v>
       </c>
       <c r="E54" s="2">
-        <v>12.569345776277697</v>
+        <v>14.196303597119659</v>
       </c>
       <c r="F54" s="2">
         <v>15.417540000000001</v>
@@ -2543,7 +2543,7 @@
         <v>2825.8794400000002</v>
       </c>
       <c r="E55" s="2">
-        <v>12.693869204837696</v>
+        <v>14.095548251697531</v>
       </c>
       <c r="F55" s="2">
         <v>13.850580000000001</v>
@@ -2566,7 +2566,7 @@
         <v>2823.0671600000001</v>
       </c>
       <c r="E56" s="2">
-        <v>12.817518659386055</v>
+        <v>13.876988317911643</v>
       </c>
       <c r="F56" s="2">
         <v>15.8894</v>
@@ -2589,7 +2589,7 @@
         <v>2806.6736099999998</v>
       </c>
       <c r="E57" s="2">
-        <v>12.312247807111424</v>
+        <v>13.26133892711522</v>
       </c>
       <c r="F57" s="2">
         <v>16.842459999999999</v>
@@ -2612,7 +2612,7 @@
         <v>2799.7305200000001</v>
       </c>
       <c r="E58" s="2">
-        <v>11.616958049233967</v>
+        <v>12.53677443213356</v>
       </c>
       <c r="F58" s="2">
         <v>16.608750000000001</v>
@@ -2635,7 +2635,7 @@
         <v>2810.0133599999999</v>
       </c>
       <c r="E59" s="2">
-        <v>10.941989258015486</v>
+        <v>11.745485081964164</v>
       </c>
       <c r="F59" s="2">
         <v>16.805479999999999</v>
@@ -2658,7 +2658,7 @@
         <v>2790.9003499999999</v>
       </c>
       <c r="E60" s="2">
-        <v>10.494726191137566</v>
+        <v>11.265332350544153</v>
       </c>
       <c r="F60" s="2">
         <v>18.027940000000001</v>
@@ -2681,7 +2681,7 @@
         <v>2779.8141500000002</v>
       </c>
       <c r="E61" s="2">
-        <v>10.245654372253627</v>
+        <v>10.959380144172586</v>
       </c>
       <c r="F61" s="2">
         <v>16.182749999999999</v>
@@ -2704,7 +2704,7 @@
         <v>2762.2802000000001</v>
       </c>
       <c r="E62" s="2">
-        <v>9.7745768151978201</v>
+        <v>10.501574025690804</v>
       </c>
       <c r="F62" s="2">
         <v>16.931819999999998</v>
@@ -2727,7 +2727,7 @@
         <v>2760.1368200000002</v>
       </c>
       <c r="E63" s="2">
-        <v>9.1788138241639761</v>
+        <v>9.879481264265733</v>
       </c>
       <c r="F63" s="2">
         <v>18.55444</v>
@@ -2750,7 +2750,7 @@
         <v>2781.68631</v>
       </c>
       <c r="E64" s="2">
-        <v>9.1758840341706254</v>
+        <v>9.7921573335132805</v>
       </c>
       <c r="F64" s="2">
         <v>19.489470000000001</v>
@@ -2773,7 +2773,7 @@
         <v>2785.5196999999998</v>
       </c>
       <c r="E65" s="2">
-        <v>8.9330798845184987</v>
+        <v>9.5002236027984317</v>
       </c>
       <c r="F65" s="2">
         <v>20.851459999999999</v>
@@ -2796,7 +2796,7 @@
         <v>2790.9014299999999</v>
       </c>
       <c r="E66" s="2">
-        <v>8.8327530076904228</v>
+        <v>9.3749925091406752</v>
       </c>
       <c r="F66" s="2">
         <v>23.526679999999999</v>
@@ -2819,7 +2819,7 @@
         <v>2786.5026200000002</v>
       </c>
       <c r="E67" s="2">
-        <v>8.4341431554081936</v>
+        <v>8.9499036609554654</v>
       </c>
       <c r="F67" s="2">
         <v>21.188590000000001</v>
@@ -2842,7 +2842,7 @@
         <v>2806.2199000000001</v>
       </c>
       <c r="E68" s="2">
-        <v>8.2778936889443333</v>
+        <v>8.7883561797847705</v>
       </c>
       <c r="F68" s="2">
         <v>18.063929999999999</v>
@@ -2865,7 +2865,7 @@
         <v>2796.0770699999998</v>
       </c>
       <c r="E69" s="2">
-        <v>7.9715996526519213</v>
+        <v>8.4774415749563019</v>
       </c>
       <c r="F69" s="2">
         <v>18.430420000000002</v>
@@ -2888,7 +2888,7 @@
         <v>2808.6781900000001</v>
       </c>
       <c r="E70" s="2">
-        <v>7.6223111199506981</v>
+        <v>8.1002124348037192</v>
       </c>
       <c r="F70" s="2">
         <v>18.745650000000001</v>
@@ -2911,7 +2911,7 @@
         <v>2792.55897</v>
       </c>
       <c r="E71" s="2">
-        <v>7.3228881537280479</v>
+        <v>7.8042935651955094</v>
       </c>
       <c r="F71" s="2">
         <v>14.1904</v>
@@ -2934,7 +2934,7 @@
         <v>2798.7469999999998</v>
       </c>
       <c r="E72" s="2">
-        <v>6.9398734505119615</v>
+        <v>7.4229003193214682</v>
       </c>
       <c r="F72" s="2">
         <v>13.34919</v>
@@ -2957,7 +2957,7 @@
         <v>2808.0852500000001</v>
       </c>
       <c r="E73" s="2">
-        <v>6.7937485160039213</v>
+        <v>7.2846898077613575</v>
       </c>
       <c r="F73" s="2">
         <v>12.4283</v>
@@ -2980,7 +2980,7 @@
         <v>2820.3229299999998</v>
       </c>
       <c r="E74" s="2">
-        <v>6.5143579143257897</v>
+        <v>7.0069848348891002</v>
       </c>
       <c r="F74" s="2">
         <v>11.23766</v>
@@ -3003,7 +3003,7 @@
         <v>2818.96486</v>
       </c>
       <c r="E75" s="2">
-        <v>6.5359402883794733</v>
+        <v>7.045742315496617</v>
       </c>
       <c r="F75" s="2">
         <v>11.300319999999999</v>
@@ -3026,7 +3026,7 @@
         <v>2814.78215</v>
       </c>
       <c r="E76" s="2">
-        <v>6.5434245772803408</v>
+        <v>7.055582153161609</v>
       </c>
       <c r="F76" s="2">
         <v>15.47588</v>
@@ -3049,7 +3049,7 @@
         <v>2824.8520400000002</v>
       </c>
       <c r="E77" s="2">
-        <v>6.4616850162530977</v>
+        <v>6.9639247733271308</v>
       </c>
       <c r="F77" s="2">
         <v>20.623950000000001</v>
@@ -3072,7 +3072,7 @@
         <v>2826.1518799999999</v>
       </c>
       <c r="E78" s="2">
-        <v>6.4485877170904207</v>
+        <v>6.9371792688852425</v>
       </c>
       <c r="F78" s="2">
         <v>24.06193</v>
@@ -3095,7 +3095,7 @@
         <v>2841.4554199999998</v>
       </c>
       <c r="E79" s="2">
-        <v>6.3954123552640505</v>
+        <v>6.8577363507956592</v>
       </c>
       <c r="F79" s="2">
         <v>26.854669999999999</v>
@@ -3118,7 +3118,7 @@
         <v>2832.9541399999998</v>
       </c>
       <c r="E80" s="2">
-        <v>6.3115483401365617</v>
+        <v>6.816208454290952</v>
       </c>
       <c r="F80" s="2">
         <v>26.7271</v>
@@ -3141,7 +3141,7 @@
         <v>2837.2400200000002</v>
       </c>
       <c r="E81" s="2">
-        <v>6.2180471428709083</v>
+        <v>6.7152332055147204</v>
       </c>
       <c r="F81" s="2">
         <v>30.611660000000001</v>
@@ -3164,7 +3164,7 @@
         <v>2833.5366399999998</v>
       </c>
       <c r="E82" s="2">
-        <v>6.0981900343452065</v>
+        <v>6.6085994552788376</v>
       </c>
       <c r="F82" s="2">
         <v>29.536709999999999</v>
@@ -3187,7 +3187,7 @@
         <v>2855.3015300000002</v>
       </c>
       <c r="E83" s="2">
-        <v>5.9943003287642265</v>
+        <v>6.5081409987502559</v>
       </c>
       <c r="F83" s="2">
         <v>25.82788</v>
@@ -3210,7 +3210,7 @@
         <v>2856.8195099999998</v>
       </c>
       <c r="E84" s="2">
-        <v>5.8449334098813965</v>
+        <v>6.3410173827293459</v>
       </c>
       <c r="F84" s="2">
         <v>27.325980000000001</v>
@@ -3233,7 +3233,7 @@
         <v>2846.2370900000001</v>
       </c>
       <c r="E85" s="2">
-        <v>5.7682739634314864</v>
+        <v>6.2614318653266636</v>
       </c>
       <c r="F85" s="2">
         <v>25.315059999999999</v>
@@ -3256,7 +3256,7 @@
         <v>2852.8621600000001</v>
       </c>
       <c r="E86" s="2">
-        <v>5.6851506278172241</v>
+        <v>6.2068696565408432</v>
       </c>
       <c r="F86" s="2">
         <v>19.338339999999999</v>
@@ -3279,7 +3279,7 @@
         <v>2855.0302999999999</v>
       </c>
       <c r="E87" s="2">
-        <v>5.8142513233572339</v>
+        <v>6.3369830026636418</v>
       </c>
       <c r="F87" s="2">
         <v>21.127680000000002</v>
@@ -3302,7 +3302,7 @@
         <v>2859.4812700000002</v>
       </c>
       <c r="E88" s="2">
-        <v>5.7718764844366337</v>
+        <v>6.2981914739625182</v>
       </c>
       <c r="F88" s="2">
         <v>25.051449999999999</v>
@@ -3325,7 +3325,7 @@
         <v>2858.4651899999999</v>
       </c>
       <c r="E89" s="2">
-        <v>5.8254555830361534</v>
+        <v>6.3568732518565891</v>
       </c>
       <c r="F89" s="2">
         <v>26.989660000000001</v>
@@ -3348,7 +3348,7 @@
         <v>2857.7744699999998</v>
       </c>
       <c r="E90" s="2">
-        <v>5.9463690289038107</v>
+        <v>6.4607079482411676</v>
       </c>
       <c r="F90" s="2">
         <v>26.779949999999999</v>
@@ -3380,7 +3380,7 @@
         <v>2849.2044599999999</v>
       </c>
       <c r="E91" s="2">
-        <v>6.2035009940985422</v>
+        <v>6.6957331541422871</v>
       </c>
       <c r="F91" s="2">
         <v>31.466339999999999</v>
@@ -3412,7 +3412,7 @@
         <v>2844.8296</v>
       </c>
       <c r="E92" s="2">
-        <v>6.4121893276138584</v>
+        <v>6.8818001381073204</v>
       </c>
       <c r="F92" s="2">
         <v>26.136289999999999</v>
@@ -3444,7 +3444,7 @@
         <v>2847.51073</v>
       </c>
       <c r="E93" s="2">
-        <v>6.4983613599938925</v>
+        <v>6.9576311970777844</v>
       </c>
       <c r="F93" s="2">
         <v>28.475020000000001</v>
@@ -3476,7 +3476,7 @@
         <v>2843.00936</v>
       </c>
       <c r="E94" s="2">
-        <v>6.6972642327143106</v>
+        <v>7.1864791272529107</v>
       </c>
       <c r="F94" s="2">
         <v>29.448460000000001</v>
@@ -3508,7 +3508,7 @@
         <v>2822.2287000000001</v>
       </c>
       <c r="E95" s="2">
-        <v>6.6127314203841809</v>
+        <v>7.1594108636132745</v>
       </c>
       <c r="F95" s="2">
         <v>31.978870000000001</v>
@@ -3540,7 +3540,7 @@
         <v>2836.2442999999998</v>
       </c>
       <c r="E96" s="2">
-        <v>6.5057569970259621</v>
+        <v>7.12020891816094</v>
       </c>
       <c r="F96" s="2">
         <v>35.449710000000003</v>
@@ -3572,7 +3572,7 @@
         <v>2826.07357</v>
       </c>
       <c r="E97" s="2">
-        <v>6.36558548615562</v>
+        <v>7.0359392186195402</v>
       </c>
       <c r="F97" s="2">
         <v>41.434539999999998</v>
@@ -3604,7 +3604,7 @@
         <v>2835.8275899999999</v>
       </c>
       <c r="E98" s="2">
-        <v>6.3522677343018588</v>
+        <v>6.9653373249724035</v>
       </c>
       <c r="F98" s="2">
         <v>44.338859999999997</v>
@@ -3636,7 +3636,7 @@
         <v>2841.0472399999999</v>
       </c>
       <c r="E99" s="2">
-        <v>6.0885834830398675</v>
+        <v>6.6511742249064847</v>
       </c>
       <c r="F99" s="2">
         <v>47.532089999999997</v>
@@ -3668,7 +3668,7 @@
         <v>2852.6362899999999</v>
       </c>
       <c r="E100" s="2">
-        <v>5.9360938719601029</v>
+        <v>6.4407859418667686</v>
       </c>
       <c r="F100" s="2">
         <v>51.044429999999998</v>
@@ -3700,7 +3700,7 @@
         <v>2849.67569</v>
       </c>
       <c r="E101" s="2">
-        <v>5.6731455641536526</v>
+        <v>6.1458794013623299</v>
       </c>
       <c r="F101" s="2">
         <v>61.570360000000001</v>
@@ -3732,7 +3732,7 @@
         <v>2850.3584099999998</v>
       </c>
       <c r="E102" s="2">
-        <v>5.3889597694487836</v>
+        <v>5.8520645424171738</v>
       </c>
       <c r="F102" s="2">
         <v>56.611809999999998</v>
@@ -3764,7 +3764,7 @@
         <v>2859.2962600000001</v>
       </c>
       <c r="E103" s="2">
-        <v>4.9167361901840847</v>
+        <v>5.3734933067016764</v>
       </c>
       <c r="F103" s="2">
         <v>61.310920000000003</v>
@@ -3796,7 +3796,7 @@
         <v>2867.7513899999999</v>
       </c>
       <c r="E104" s="2">
-        <v>4.6154536429324162</v>
+        <v>5.0440390722918016</v>
       </c>
       <c r="F104" s="2">
         <v>69.359390000000005</v>
@@ -3828,7 +3828,7 @@
         <v>2869.7239199999999</v>
       </c>
       <c r="E105" s="2">
-        <v>4.3597538469833017</v>
+        <v>4.7540041595148832</v>
       </c>
       <c r="F105" s="2">
         <v>69.673569999999998</v>
@@ -3860,7 +3860,7 @@
         <v>2882.3636700000002</v>
       </c>
       <c r="E106" s="2">
-        <v>4.0321934462905578</v>
+        <v>4.3711649036526108</v>
       </c>
       <c r="F106" s="2">
         <v>59.699069999999999</v>
@@ -3892,7 +3892,7 @@
         <v>2910.2888499999999</v>
       </c>
       <c r="E107" s="2">
-        <v>3.6895868600809156</v>
+        <v>3.9527389842365315</v>
       </c>
       <c r="F107" s="2">
         <v>57.912750000000003</v>
@@ -3924,7 +3924,7 @@
         <v>2905.9630200000001</v>
       </c>
       <c r="E108" s="2">
-        <v>3.4266266196326196</v>
+        <v>3.644704763095461</v>
       </c>
       <c r="F108" s="2">
         <v>68.722970000000004</v>
@@ -3956,7 +3956,7 @@
         <v>2891.9307899999999</v>
       </c>
       <c r="E109" s="2">
-        <v>3.1614186901063426</v>
+        <v>3.3594114429074908</v>
       </c>
       <c r="F109" s="2">
         <v>75.002520000000004</v>
@@ -3988,7 +3988,7 @@
         <v>2886.13762</v>
       </c>
       <c r="E110" s="2">
-        <v>2.8069432704321282</v>
+        <v>3.0036122973347275</v>
       </c>
       <c r="F110" s="2">
         <v>88.710530000000006</v>
@@ -4020,7 +4020,7 @@
         <v>2907.96992</v>
       </c>
       <c r="E111" s="2">
-        <v>2.4302147561416314</v>
+        <v>2.6258321009016159</v>
       </c>
       <c r="F111" s="2">
         <v>96.946950000000001</v>
@@ -4052,7 +4052,7 @@
         <v>2898.1729099999998</v>
       </c>
       <c r="E112" s="2">
-        <v>2.1363844643762131</v>
+        <v>2.3320259211446559</v>
       </c>
       <c r="F112" s="2">
         <v>121.7448</v>
@@ -4084,7 +4084,7 @@
         <v>2911.3177900000001</v>
       </c>
       <c r="E113" s="2">
-        <v>2.1794867368292352</v>
+        <v>2.3832927862592572</v>
       </c>
       <c r="F113" s="2">
         <v>115.06059999999999</v>
@@ -4116,7 +4116,7 @@
         <v>2914.9343399999998</v>
       </c>
       <c r="E114" s="2">
-        <v>2.5051245819828658</v>
+        <v>2.7190902719148351</v>
       </c>
       <c r="F114" s="2">
         <v>54.877940000000002</v>
@@ -4148,7 +4148,7 @@
         <v>2884.3014400000002</v>
       </c>
       <c r="E115" s="2">
-        <v>3.240385311460372</v>
+        <v>3.4661989843215362</v>
       </c>
       <c r="F115" s="2">
         <v>44.456760000000003</v>
@@ -4180,7 +4180,7 @@
         <v>2875.19607</v>
       </c>
       <c r="E116" s="2">
-        <v>4.1909552276203552</v>
+        <v>4.449208249324256</v>
       </c>
       <c r="F116" s="2">
         <v>58.95946</v>
@@ -4212,7 +4212,7 @@
         <v>2870.6467600000001</v>
       </c>
       <c r="E117" s="2">
-        <v>4.6856175365860757</v>
+        <v>4.9953569495687837</v>
       </c>
       <c r="F117" s="2">
         <v>68.321520000000007</v>
@@ -4244,7 +4244,7 @@
         <v>2857.07573</v>
       </c>
       <c r="E118" s="2">
-        <v>5.0660439091686245</v>
+        <v>5.4413415545346018</v>
       </c>
       <c r="F118" s="2">
         <v>74.735050000000001</v>
@@ -4276,7 +4276,7 @@
         <v>2829.8395799999998</v>
       </c>
       <c r="E119" s="2">
-        <v>5.2813742537306663</v>
+        <v>5.7427722119205216</v>
       </c>
       <c r="F119" s="2">
         <v>76.365070000000003</v>
@@ -4308,7 +4308,7 @@
         <v>2832.2677399999998</v>
       </c>
       <c r="E120" s="2">
-        <v>5.2045649822640012</v>
+        <v>5.7541915107552537</v>
       </c>
       <c r="F120" s="2">
         <v>78.353970000000004</v>
@@ -4340,7 +4340,7 @@
         <v>2833.35581</v>
       </c>
       <c r="E121" s="2">
-        <v>5.1901437680712608</v>
+        <v>5.8123351320126782</v>
       </c>
       <c r="F121" s="2">
         <v>76.850610000000003</v>
@@ -4372,7 +4372,7 @@
         <v>2832.78611</v>
       </c>
       <c r="E122" s="2">
-        <v>5.1398669135665873</v>
+        <v>5.7699511228486458</v>
       </c>
       <c r="F122" s="2">
         <v>86.580510000000004</v>
@@ -4404,7 +4404,7 @@
         <v>2823.5940599999999</v>
       </c>
       <c r="E123" s="2">
-        <v>5.0542014527399877</v>
+        <v>5.7024813493993864</v>
       </c>
       <c r="F123" s="2">
         <v>104.91370000000001</v>
@@ -4436,7 +4436,7 @@
         <v>2831.3271399999999</v>
       </c>
       <c r="E124" s="2">
-        <v>4.9691655906636063</v>
+        <v>5.6299286408439775</v>
       </c>
       <c r="F124" s="2">
         <v>117.49379999999999</v>
@@ -4468,7 +4468,7 @@
         <v>2832.87635</v>
       </c>
       <c r="E125" s="2">
-        <v>4.9815019635431668</v>
+        <v>5.6296464656788805</v>
       </c>
       <c r="F125" s="2">
         <v>113.1405</v>
@@ -4500,7 +4500,7 @@
         <v>2831.4003600000001</v>
       </c>
       <c r="E126" s="2">
-        <v>4.9146451334067072</v>
+        <v>5.5422858778230815</v>
       </c>
       <c r="F126" s="2">
         <v>109.4419</v>
@@ -4532,7 +4532,7 @@
         <v>2822.47318</v>
       </c>
       <c r="E127" s="2">
-        <v>5.0574783141074882</v>
+        <v>5.6697380203176131</v>
       </c>
       <c r="F127" s="2">
         <v>118.6489</v>
@@ -4564,7 +4564,7 @@
         <v>2823.90229</v>
       </c>
       <c r="E128" s="2">
-        <v>5.2756717017995687</v>
+        <v>5.8229116673529546</v>
       </c>
       <c r="F128" s="2">
         <v>108.8227</v>
@@ -4596,7 +4596,7 @@
         <v>2821.3447099999998</v>
       </c>
       <c r="E129" s="2">
-        <v>5.28845275343898</v>
+        <v>5.7697722340383848</v>
       </c>
       <c r="F129" s="2">
         <v>109.6541</v>
@@ -4628,7 +4628,7 @@
         <v>2820.65924</v>
       </c>
       <c r="E130" s="2">
-        <v>5.2272635031234751</v>
+        <v>5.6922298817276111</v>
       </c>
       <c r="F130" s="2">
         <v>110.2563</v>
@@ -4660,7 +4660,7 @@
         <v>2818.7222499999998</v>
       </c>
       <c r="E131" s="2">
-        <v>5.1687270712820323</v>
+        <v>5.57363532695567</v>
       </c>
       <c r="F131" s="2">
         <v>112.6075</v>
@@ -4692,7 +4692,7 @@
         <v>2820.61384</v>
       </c>
       <c r="E132" s="2">
-        <v>5.1683524675607497</v>
+        <v>5.5250267475536461</v>
       </c>
       <c r="F132" s="2">
         <v>102.70269999999999</v>
@@ -4724,7 +4724,7 @@
         <v>2824.6955800000001</v>
       </c>
       <c r="E133" s="2">
-        <v>5.0250938899405222</v>
+        <v>5.3621318501364899</v>
       </c>
       <c r="F133" s="2">
         <v>110.3498</v>
@@ -4756,7 +4756,7 @@
         <v>2826.7089099999998</v>
       </c>
       <c r="E134" s="2">
-        <v>4.9235672448494183</v>
+        <v>5.2547523638473717</v>
       </c>
       <c r="F134" s="2">
         <v>109.32810000000001</v>
@@ -4788,7 +4788,7 @@
         <v>2822.3292499999998</v>
       </c>
       <c r="E135" s="2">
-        <v>4.622420435177788</v>
+        <v>4.9062624101196848</v>
       </c>
       <c r="F135" s="2">
         <v>108.24769999999999</v>
@@ -4820,7 +4820,7 @@
         <v>2825.7004499999998</v>
       </c>
       <c r="E136" s="2">
-        <v>4.4940921816394228</v>
+        <v>4.7503453327426248</v>
       </c>
       <c r="F136" s="2">
         <v>109.7867</v>
@@ -4852,7 +4852,7 @@
         <v>2827.5064200000002</v>
       </c>
       <c r="E137" s="2">
-        <v>4.4211980250782243</v>
+        <v>4.6556395133728703</v>
       </c>
       <c r="F137" s="2">
         <v>101.9479</v>
@@ -4884,7 +4884,7 @@
         <v>2833.9921599999998</v>
       </c>
       <c r="E138" s="2">
-        <v>4.3528913290995135</v>
+        <v>4.5579586012179902</v>
       </c>
       <c r="F138" s="2">
         <v>76.053849999999997</v>
@@ -4916,7 +4916,7 @@
         <v>2845.0744</v>
       </c>
       <c r="E139" s="2">
-        <v>4.2971153935376876</v>
+        <v>4.4764577222344917</v>
       </c>
       <c r="F139" s="2">
         <v>54.198030000000003</v>
@@ -4948,7 +4948,7 @@
         <v>2853.6372000000001</v>
       </c>
       <c r="E140" s="2">
-        <v>4.2530013275689003</v>
+        <v>4.4082806462605255</v>
       </c>
       <c r="F140" s="2">
         <v>61.675660000000001</v>
@@ -4980,7 +4980,7 @@
         <v>2858.2902300000001</v>
       </c>
       <c r="E141" s="2">
-        <v>4.0765532407113181</v>
+        <v>4.2106902570718132</v>
       </c>
       <c r="F141" s="2">
         <v>50.198349999999998</v>
@@ -5012,7 +5012,7 @@
         <v>2865.5751300000002</v>
       </c>
       <c r="E142" s="2">
-        <v>3.9571706500677228</v>
+        <v>4.0853816116326671</v>
       </c>
       <c r="F142" s="2">
         <v>43.543370000000003</v>
@@ -5044,7 +5044,7 @@
         <v>2876.30951</v>
       </c>
       <c r="E143" s="2">
-        <v>3.8587625780231138</v>
+        <v>3.9837465754529235</v>
       </c>
       <c r="F143" s="2">
         <v>33.929139999999997</v>
@@ -5076,7 +5076,7 @@
         <v>2884.0498400000001</v>
       </c>
       <c r="E144" s="2">
-        <v>3.7541571056899627</v>
+        <v>3.8803774440109589</v>
       </c>
       <c r="F144" s="2">
         <v>45.539479999999998</v>
@@ -5108,7 +5108,7 @@
         <v>2896.1749799999998</v>
       </c>
       <c r="E145" s="2">
-        <v>3.7045164998973932</v>
+        <v>3.8283394976019887</v>
       </c>
       <c r="F145" s="2">
         <v>45.750070000000001</v>
@@ -5140,7 +5140,7 @@
         <v>2909.7444700000001</v>
       </c>
       <c r="E146" s="2">
-        <v>3.7519650995332929</v>
+        <v>3.8708688400446638</v>
       </c>
       <c r="F146" s="2">
         <v>49.303359999999998</v>
@@ -5172,7 +5172,7 @@
         <v>2921.6062000000002</v>
       </c>
       <c r="E147" s="2">
-        <v>3.8453094397184668</v>
+        <v>3.9676867751913849</v>
       </c>
       <c r="F147" s="2">
         <v>53.662190000000002</v>
@@ -5204,7 +5204,7 @@
         <v>2933.3497299999999</v>
       </c>
       <c r="E148" s="2">
-        <v>3.8396925142642298</v>
+        <v>3.9622381179284556</v>
       </c>
       <c r="F148" s="2">
         <v>49.734760000000001</v>
@@ -5236,7 +5236,7 @@
         <v>2942.2687799999999</v>
       </c>
       <c r="E149" s="2">
-        <v>3.8971812425647943</v>
+        <v>4.0160358653203998</v>
       </c>
       <c r="F149" s="2">
         <v>52.054220000000001</v>
@@ -5268,7 +5268,7 @@
         <v>2950.5178900000001</v>
       </c>
       <c r="E150" s="2">
-        <v>3.7878700338942868</v>
+        <v>3.8986440152373172</v>
       </c>
       <c r="F150" s="2">
         <v>61.766249999999999</v>
@@ -5300,7 +5300,7 @@
         <v>2956.7958100000001</v>
       </c>
       <c r="E151" s="2">
-        <v>3.6657910780792129</v>
+        <v>3.7734489879035298</v>
       </c>
       <c r="F151" s="2">
         <v>66.880619999999993</v>
@@ -5332,7 +5332,7 @@
         <v>2965.7101699999998</v>
       </c>
       <c r="E152" s="2">
-        <v>3.5616764601107334</v>
+        <v>3.6630618223935527</v>
       </c>
       <c r="F152" s="2">
         <v>74.449010000000001</v>
@@ -5364,7 +5364,7 @@
         <v>2977.1850300000001</v>
       </c>
       <c r="E153" s="2">
-        <v>3.4736079873409813</v>
+        <v>3.5689718088789562</v>
       </c>
       <c r="F153" s="2">
         <v>75.207830000000001</v>
@@ -5396,7 +5396,7 @@
         <v>2982.19497</v>
       </c>
       <c r="E154" s="2">
-        <v>3.459335725457279</v>
+        <v>3.5473057148546587</v>
       </c>
       <c r="F154" s="2">
         <v>67.102980000000002</v>
@@ -5428,7 +5428,7 @@
         <v>2991.3098</v>
       </c>
       <c r="E155" s="2">
-        <v>3.3831213336712898</v>
+        <v>3.4672825696562217</v>
       </c>
       <c r="F155" s="2">
         <v>63.22681</v>
@@ -5460,7 +5460,7 @@
         <v>2997.7643200000002</v>
       </c>
       <c r="E156" s="2">
-        <v>3.3325647994903078</v>
+        <v>3.4177016282366282</v>
       </c>
       <c r="F156" s="2">
         <v>69.061750000000004</v>
@@ -5492,7 +5492,7 @@
         <v>3009.72894</v>
       </c>
       <c r="E157" s="2">
-        <v>3.3965835142615872</v>
+        <v>3.4744363317579894</v>
       </c>
       <c r="F157" s="2">
         <v>61.9816</v>
@@ -5524,7 +5524,7 @@
         <v>3015.1360800000002</v>
       </c>
       <c r="E158" s="2">
-        <v>3.4514286665297038</v>
+        <v>3.5257334385460801</v>
       </c>
       <c r="F158" s="2">
         <v>63.43647</v>
@@ -5556,7 +5556,7 @@
         <v>3019.2933499999999</v>
       </c>
       <c r="E159" s="2">
-        <v>3.5164810335504497</v>
+        <v>3.5896862146652184</v>
       </c>
       <c r="F159" s="2">
         <v>50.550109999999997</v>
@@ -5588,7 +5588,7 @@
         <v>2990.16824</v>
       </c>
       <c r="E160" s="2">
-        <v>4.9974567317322593</v>
+        <v>5.0403698146161284</v>
       </c>
       <c r="F160" s="2">
         <v>29.529540000000001</v>
@@ -5620,7 +5620,7 @@
         <v>3022.3491899999999</v>
       </c>
       <c r="E161" s="2">
-        <v>4.5512441598450772</v>
+        <v>4.5961475591544216</v>
       </c>
       <c r="F161" s="2">
         <v>42.956150000000001</v>
@@ -5652,7 +5652,7 @@
         <v>3026.1817500000002</v>
       </c>
       <c r="E162" s="2">
-        <v>4.2678014630152337</v>
+        <v>4.3387358778403957</v>
       </c>
       <c r="F162" s="2">
         <v>44.269300000000001</v>
@@ -5684,7 +5684,7 @@
         <v>3011.9945400000001</v>
       </c>
       <c r="E163" s="2">
-        <v>4.2137974459940422</v>
+        <v>4.2723363428582299</v>
       </c>
       <c r="F163" s="2">
         <v>60.775880000000001</v>
@@ -5716,7 +5716,7 @@
         <v>3053.2020299999999</v>
       </c>
       <c r="E164" s="2">
-        <v>3.7037591646039885</v>
+        <v>3.7482590683204191</v>
       </c>
       <c r="F164" s="2">
         <v>68.796099999999996</v>
@@ -5748,7 +5748,7 @@
         <v>3087.7042200000001</v>
       </c>
       <c r="E165" s="2">
-        <v>3.0765743779694028</v>
+        <v>3.1359481291026938</v>
       </c>
       <c r="F165" s="2">
         <v>73.461669999999998</v>
@@ -5780,7 +5780,7 @@
         <v>3105.1590500000002</v>
       </c>
       <c r="E166" s="2">
-        <v>2.5331168334195313</v>
+        <v>2.5759045556827318</v>
       </c>
       <c r="F166" s="2">
         <v>79.462999999999994</v>
@@ -5812,7 +5812,7 @@
         <v>3110.4208899999999</v>
       </c>
       <c r="E167" s="2">
-        <v>2.3266001920402486</v>
+        <v>2.365946693770741</v>
       </c>
       <c r="F167" s="2">
         <v>101.04073015873014</v>

</xml_diff>